<commit_message>
updated fuel and ccs files from RMI
</commit_message>
<xml_diff>
--- a/InputData/ccs/BFoCPAbS/BAU Fraction of CCS Potential Achieved by Sector.xlsx
+++ b/InputData/ccs/BFoCPAbS/BAU Fraction of CCS Potential Achieved by Sector.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepositories\eps-us\InputData\ccs\BFoCPAbS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nathaniyer/Library/Containers/com.microsoft.Excel/Data/state-eps-data-repository/MN/ccs/BFoCPAbS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8172C6A6-BBA0-434B-9A8B-7CEBCD3A7416}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{875C29CB-C0C7-7A48-8327-FABDF44891A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="171">
   <si>
     <t>Source:</t>
   </si>
@@ -569,6 +569,9 @@
   </si>
   <si>
     <t>https://co2re.co/FacilityData</t>
+  </si>
+  <si>
+    <t>Minnesota</t>
   </si>
 </sst>
 </file>
@@ -7399,20 +7402,23 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="103.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="103.5" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" customWidth="1"/>
+    <col min="4" max="4" width="22.1640625" customWidth="1"/>
+    <col min="5" max="5" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -7420,83 +7426,83 @@
         <v>167</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4" s="34">
         <v>2020</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B6" s="35" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" s="8"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="3"/>
       <c r="C16" s="4"/>
       <c r="D16" s="5"/>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="3"/>
       <c r="C18" s="4"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B19" s="3"/>
       <c r="C19" s="4"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B20" s="3"/>
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
     </row>
@@ -7515,45 +7521,45 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.85546875" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" customWidth="1"/>
+    <col min="1" max="1" width="35.83203125" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" customWidth="1"/>
+    <col min="5" max="5" width="9.5" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="86.42578125" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" style="25" customWidth="1"/>
-    <col min="10" max="10" width="25.5703125" customWidth="1"/>
+    <col min="7" max="7" width="86.5" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" style="25" customWidth="1"/>
+    <col min="10" max="10" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -7585,7 +7591,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>21</v>
       </c>
@@ -7618,7 +7624,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>26</v>
       </c>
@@ -7651,7 +7657,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>29</v>
       </c>
@@ -7684,7 +7690,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
         <v>31</v>
       </c>
@@ -7717,7 +7723,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>34</v>
       </c>
@@ -7750,7 +7756,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>36</v>
       </c>
@@ -7783,7 +7789,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
         <v>38</v>
       </c>
@@ -7815,7 +7821,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
         <v>43</v>
       </c>
@@ -7848,7 +7854,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
         <v>46</v>
       </c>
@@ -7880,7 +7886,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
         <v>50</v>
       </c>
@@ -7913,7 +7919,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
         <v>52</v>
       </c>
@@ -7946,7 +7952,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
         <v>54</v>
       </c>
@@ -7979,7 +7985,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
         <v>57</v>
       </c>
@@ -8012,7 +8018,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
         <v>59</v>
       </c>
@@ -8046,7 +8052,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
         <v>61</v>
       </c>
@@ -8079,7 +8085,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
         <v>63</v>
       </c>
@@ -8112,7 +8118,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
         <v>65</v>
       </c>
@@ -8146,7 +8152,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
         <v>67</v>
       </c>
@@ -8179,7 +8185,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
         <v>70</v>
       </c>
@@ -8211,7 +8217,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
         <v>74</v>
       </c>
@@ -8244,7 +8250,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
         <v>76</v>
       </c>
@@ -8277,7 +8283,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
         <v>78</v>
       </c>
@@ -8309,7 +8315,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
         <v>81</v>
       </c>
@@ -8343,7 +8349,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
         <v>83</v>
       </c>
@@ -8376,7 +8382,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
         <v>85</v>
       </c>
@@ -8409,7 +8415,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
         <v>88</v>
       </c>
@@ -8442,7 +8448,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
         <v>90</v>
       </c>
@@ -8473,7 +8479,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
         <v>92</v>
       </c>
@@ -8506,7 +8512,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
         <v>94</v>
       </c>
@@ -8552,13 +8558,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="53.5703125" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53.5" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>101</v>
       </c>
@@ -8596,7 +8602,7 @@
       <c r="AG1" s="7"/>
       <c r="AH1" s="7"/>
     </row>
-    <row r="2" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="23"/>
       <c r="B2" s="36">
         <v>2018</v>
@@ -8698,7 +8704,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="3" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="30" t="s">
         <v>116</v>
       </c>
@@ -8835,7 +8841,7 @@
         <v>6400000</v>
       </c>
     </row>
-    <row r="4" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="30" t="s">
         <v>117</v>
       </c>
@@ -8972,7 +8978,7 @@
         <v>1400000</v>
       </c>
     </row>
-    <row r="5" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="31" t="s">
         <v>133</v>
       </c>
@@ -9109,7 +9115,7 @@
         <v>20854761.904761903</v>
       </c>
     </row>
-    <row r="6" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="31" t="s">
         <v>135</v>
       </c>
@@ -9246,7 +9252,7 @@
         <v>9065000</v>
       </c>
     </row>
-    <row r="7" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="31" t="s">
         <v>139</v>
       </c>
@@ -9383,63 +9389,63 @@
         <v>2283333.3333333335</v>
       </c>
     </row>
-    <row r="8" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="17"/>
     </row>
-    <row r="17" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="17"/>
     </row>
-    <row r="18" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="26" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="17"/>
     </row>
-    <row r="27" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="28" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="29" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="30" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="31" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="17"/>
     </row>
-    <row r="32" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="17"/>
       <c r="B32" s="36">
         <v>2018</v>
@@ -9541,7 +9547,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="33" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="30" t="s">
         <v>116</v>
       </c>
@@ -9678,7 +9684,7 @@
         <v>17191111.111110926</v>
       </c>
     </row>
-    <row r="34" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="30" t="s">
         <v>117</v>
       </c>
@@ -9815,7 +9821,7 @@
         <v>1400000</v>
       </c>
     </row>
-    <row r="35" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:34" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="31" t="s">
         <v>133</v>
       </c>
@@ -9952,7 +9958,7 @@
         <v>20854761.904761907</v>
       </c>
     </row>
-    <row r="36" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:34" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="31" t="s">
         <v>135</v>
       </c>
@@ -10089,7 +10095,7 @@
         <v>32815000</v>
       </c>
     </row>
-    <row r="37" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:34" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="31" t="s">
         <v>139</v>
       </c>
@@ -10226,55 +10232,55 @@
         <v>3527777.777777791</v>
       </c>
     </row>
-    <row r="38" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="17"/>
     </row>
-    <row r="39" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="17"/>
     </row>
-    <row r="40" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="17"/>
     </row>
-    <row r="41" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="17"/>
     </row>
-    <row r="42" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="17"/>
     </row>
-    <row r="43" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="17"/>
     </row>
-    <row r="44" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="17"/>
     </row>
-    <row r="45" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="17"/>
     </row>
-    <row r="46" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="17"/>
     </row>
-    <row r="47" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="17"/>
     </row>
-    <row r="48" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="17"/>
     </row>
-    <row r="49" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="17"/>
     </row>
-    <row r="50" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="17"/>
     </row>
-    <row r="51" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="17"/>
     </row>
-    <row r="52" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="17"/>
     </row>
-    <row r="53" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="17"/>
     </row>
-    <row r="55" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A55" s="14" t="s">
         <v>157</v>
       </c>
@@ -10312,12 +10318,12 @@
       <c r="AG55" s="7"/>
       <c r="AH55" s="7"/>
     </row>
-    <row r="56" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="57" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="8" t="s">
         <v>100</v>
       </c>
@@ -10418,7 +10424,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="58" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="8" t="s">
         <v>141</v>
       </c>
@@ -10519,7 +10525,7 @@
         <v>957155000000000</v>
       </c>
     </row>
-    <row r="59" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="8" t="s">
         <v>142</v>
       </c>
@@ -10620,7 +10626,7 @@
         <v>344835000000000</v>
       </c>
     </row>
-    <row r="60" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="8" t="s">
         <v>143</v>
       </c>
@@ -10721,7 +10727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="8" t="s">
         <v>144</v>
       </c>
@@ -10822,7 +10828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="8" t="s">
         <v>145</v>
       </c>
@@ -10923,7 +10929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="8" t="s">
         <v>146</v>
       </c>
@@ -11024,7 +11030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="8" t="s">
         <v>147</v>
       </c>
@@ -11125,7 +11131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="8" t="s">
         <v>148</v>
       </c>
@@ -11226,7 +11232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="8" t="s">
         <v>149</v>
       </c>
@@ -11327,7 +11333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="8" t="s">
         <v>150</v>
       </c>
@@ -11428,7 +11434,7 @@
         <v>11286300000000</v>
       </c>
     </row>
-    <row r="68" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="8" t="s">
         <v>151</v>
       </c>
@@ -11529,7 +11535,7 @@
         <v>99792600000000</v>
       </c>
     </row>
-    <row r="69" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="8" t="s">
         <v>152</v>
       </c>
@@ -11630,7 +11636,7 @@
         <v>43507100000000</v>
       </c>
     </row>
-    <row r="70" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="8" t="s">
         <v>153</v>
       </c>
@@ -11731,7 +11737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="8" t="s">
         <v>154</v>
       </c>
@@ -11832,7 +11838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="8" t="s">
         <v>155</v>
       </c>
@@ -11933,7 +11939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="8" t="s">
         <v>156</v>
       </c>
@@ -12034,7 +12040,7 @@
         <v>24454600000000</v>
       </c>
     </row>
-    <row r="74" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B74" s="29"/>
       <c r="C74" s="29"/>
       <c r="D74" s="29"/>
@@ -12068,12 +12074,12 @@
       <c r="AF74" s="29"/>
       <c r="AG74" s="29"/>
     </row>
-    <row r="75" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="76" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="8" t="s">
         <v>100</v>
       </c>
@@ -12174,7 +12180,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="77" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="8" t="s">
         <v>158</v>
       </c>
@@ -12275,7 +12281,7 @@
         <v>117354000000000</v>
       </c>
     </row>
-    <row r="78" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="8" t="s">
         <v>159</v>
       </c>
@@ -12376,7 +12382,7 @@
         <v>455116000000000</v>
       </c>
     </row>
-    <row r="79" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="8" t="s">
         <v>160</v>
       </c>
@@ -12477,7 +12483,7 @@
         <v>93020200000000</v>
       </c>
     </row>
-    <row r="80" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="8" t="s">
         <v>161</v>
       </c>
@@ -12578,7 +12584,7 @@
         <v>400057000000000</v>
       </c>
     </row>
-    <row r="81" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="8" t="s">
         <v>162</v>
       </c>
@@ -12679,7 +12685,7 @@
         <v>17412300000000</v>
       </c>
     </row>
-    <row r="82" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="8" t="s">
         <v>163</v>
       </c>
@@ -12780,7 +12786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="8" t="s">
         <v>164</v>
       </c>
@@ -12881,7 +12887,7 @@
         <v>87142300000000</v>
       </c>
     </row>
-    <row r="84" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="8" t="s">
         <v>165</v>
       </c>
@@ -12982,7 +12988,7 @@
         <v>549719000000000</v>
       </c>
     </row>
-    <row r="86" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="13" t="s">
         <v>102</v>
       </c>
@@ -13020,7 +13026,7 @@
       <c r="AG86" s="7"/>
       <c r="AH86" s="7"/>
     </row>
-    <row r="87" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="23"/>
       <c r="B87">
         <v>2019</v>
@@ -13119,7 +13125,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="88" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A88" s="30" t="s">
         <v>116</v>
       </c>
@@ -13252,7 +13258,7 @@
         <v>1.7960634496096167E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A89" s="30" t="s">
         <v>117</v>
       </c>
@@ -13385,7 +13391,7 @@
         <v>4.0599127118766945E-3</v>
       </c>
     </row>
-    <row r="90" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:34" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="31" t="s">
         <v>133</v>
       </c>
@@ -13518,7 +13524,7 @@
         <v>4.5822959212073203E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:34" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="31" t="s">
         <v>135</v>
       </c>
@@ -13651,7 +13657,7 @@
         <v>8.2025811321886632E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:34" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A92" s="31" t="s">
         <v>139</v>
       </c>
@@ -13784,100 +13790,100 @@
         <v>6.4174201324272784E-3</v>
       </c>
     </row>
-    <row r="93" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A93" s="23"/>
     </row>
-    <row r="94" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A94" s="23"/>
     </row>
-    <row r="95" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A95" s="23"/>
     </row>
-    <row r="96" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A96" s="23"/>
     </row>
-    <row r="97" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A97" s="23"/>
     </row>
-    <row r="98" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A98" s="23"/>
     </row>
-    <row r="99" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A99" s="23"/>
     </row>
-    <row r="100" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A100" s="23"/>
     </row>
-    <row r="101" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A101" s="23"/>
     </row>
-    <row r="102" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A102" s="23"/>
     </row>
-    <row r="103" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A103" s="23"/>
     </row>
-    <row r="104" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A104" s="23"/>
     </row>
-    <row r="105" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A105" s="23"/>
     </row>
-    <row r="106" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A106" s="23"/>
     </row>
-    <row r="107" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A107" s="23"/>
     </row>
-    <row r="108" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A108" s="23"/>
     </row>
-    <row r="109" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A109" s="23"/>
     </row>
-    <row r="110" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A110" s="23"/>
     </row>
-    <row r="111" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A111" s="23"/>
     </row>
-    <row r="112" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A112" s="23"/>
     </row>
-    <row r="113" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A113" s="23"/>
     </row>
-    <row r="114" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A114" s="23"/>
     </row>
-    <row r="115" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="116" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="117" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="118" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" s="14" t="s">
         <v>113</v>
       </c>
       <c r="B120" s="7"/>
       <c r="C120" s="7"/>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B121">
         <v>2019</v>
       </c>
@@ -13885,7 +13891,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" s="30" t="s">
         <v>116</v>
       </c>
@@ -13898,7 +13904,7 @@
         <v>1.7960634496096167E-2</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" s="30" t="s">
         <v>117</v>
       </c>
@@ -13911,7 +13917,7 @@
         <v>4.0599127118766945E-3</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A124" s="31" t="s">
         <v>133</v>
       </c>
@@ -13927,7 +13933,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A125" s="31" t="s">
         <v>135</v>
       </c>
@@ -13940,7 +13946,7 @@
         <v>8.2025811321886632E-2</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A126" s="31" t="s">
         <v>139</v>
       </c>
@@ -13968,12 +13974,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="44.85546875" customWidth="1"/>
+    <col min="1" max="1" width="44.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>115</v>
       </c>
@@ -14074,7 +14080,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>116</v>
       </c>
@@ -14207,7 +14213,7 @@
         <v>1.7960634496096084E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>117</v>
       </c>
@@ -14340,7 +14346,7 @@
         <v>4.0599127118766953E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:33" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>125</v>
       </c>
@@ -14441,7 +14447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:33" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>126</v>
       </c>
@@ -14542,7 +14548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:33" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
         <v>127</v>
       </c>
@@ -14643,7 +14649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:33" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
         <v>128</v>
       </c>
@@ -14744,7 +14750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:33" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
         <v>129</v>
       </c>
@@ -14845,7 +14851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>118</v>
       </c>
@@ -14946,7 +14952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:33" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
         <v>130</v>
       </c>
@@ -15047,7 +15053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>119</v>
       </c>
@@ -15148,7 +15154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>120</v>
       </c>
@@ -15249,7 +15255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>121</v>
       </c>
@@ -15350,7 +15356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:33" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>131</v>
       </c>
@@ -15451,7 +15457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>122</v>
       </c>
@@ -15552,7 +15558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
         <v>123</v>
       </c>
@@ -15653,7 +15659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
         <v>124</v>
       </c>
@@ -15769,12 +15775,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="44.85546875" customWidth="1"/>
+    <col min="1" max="1" width="44.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>115</v>
       </c>
@@ -15875,7 +15881,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
         <v>132</v>
       </c>
@@ -15976,7 +15982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
         <v>133</v>
       </c>
@@ -16109,7 +16115,7 @@
         <v>5.2586784705056525E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
         <v>134</v>
       </c>
@@ -16210,7 +16216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
         <v>135</v>
       </c>
@@ -16343,7 +16349,7 @@
         <v>8.2025811321886799E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
         <v>136</v>
       </c>
@@ -16444,7 +16450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
         <v>137</v>
       </c>
@@ -16545,7 +16551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
         <v>138</v>
       </c>
@@ -16646,7 +16652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
         <v>139</v>
       </c>

</xml_diff>